<commit_message>
Refactored code, Login partial code changes, Results data population to DB, User Authentication default creds, Updated input data sheets etc.
</commit_message>
<xml_diff>
--- a/cis-util/data/research.xlsx
+++ b/cis-util/data/research.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asha\java_sourcecode\cis_project\trunk\cis-util\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Personal\code\DSCE\CeninfoSys\trunk\cis-util\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -156,17 +156,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -179,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -187,19 +176,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -544,22 +524,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="72.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" customWidth="1"/>
+    <col min="4" max="4" width="57" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -578,76 +559,6 @@
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -662,16 +573,16 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,11 +602,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -707,12 +618,12 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F3" s="6" t="s">
+    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>